<commit_message>
While IRTH Framework code
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/IRTH-TestData.xlsx
+++ b/src/test/java/TestData/IRTH-TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26707"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86818D3C-D1F9-4129-BF9D-FB5BA80A005D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A9F5B21-9920-4DE4-97FF-F91A7A490A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="InstantSearch" sheetId="1" r:id="rId1"/>
-    <sheet name="KeywordSearch" sheetId="3" r:id="rId2"/>
-    <sheet name="Login" sheetId="2" r:id="rId3"/>
+    <sheet name="Instant Search" sheetId="1" r:id="rId1"/>
+    <sheet name="Keyword Search" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,19 +34,19 @@
     <t>ProductName/SKU</t>
   </si>
   <si>
-    <t>OH SO OLIVE WORK BAG</t>
+    <t>Product Value</t>
   </si>
   <si>
-    <t>Product Keyword</t>
+    <t>Product1</t>
   </si>
   <si>
-    <t>bags</t>
+    <t>IRTH Boss Bag</t>
   </si>
   <si>
-    <t>Mobile Number</t>
+    <t>Product2</t>
   </si>
   <si>
-    <t>OTP</t>
+    <t>OH SO OLIVE WORK BAG</t>
   </si>
 </sst>
 </file>
@@ -106,9 +105,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,26 +422,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -451,64 +465,268 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB35AA7B-3981-43C5-AC02-E08BB11BD771}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F65662-224B-439C-A17C-9850671EB6E7}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B2F7C3-A59C-4903-B355-3B3208DAC185}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>7020491561</v>
-      </c>
-      <c r="B2">
-        <v>214263</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002B78F710EDC7A34DA6B0F3C9F9963B35" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d22a45f451f85d5779c5367bc9ce5b0d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fb8349a5-8f94-4106-8ba3-44e9d31faefb" xmlns:ns3="487dfd21-4f41-40d9-bb9c-27381fa7f869" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="adfa0bf2fccfb4c1860d0e17610fc107" ns2:_="" ns3:_="">
+    <xsd:import namespace="fb8349a5-8f94-4106-8ba3-44e9d31faefb"/>
+    <xsd:import namespace="487dfd21-4f41-40d9-bb9c-27381fa7f869"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb8349a5-8f94-4106-8ba3-44e9d31faefb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="12" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="14" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5866b93a-4635-4247-88ec-09744cab2739" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="20" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="487dfd21-4f41-40d9-bb9c-27381fa7f869" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="15" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{22b75d2e-b219-4cd1-8b11-0ea463775527}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="487dfd21-4f41-40d9-bb9c-27381fa7f869">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="487dfd21-4f41-40d9-bb9c-27381fa7f869" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fb8349a5-8f94-4106-8ba3-44e9d31faefb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D760C5BD-69B8-43AA-9809-BE2E5142614E}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ABF829A-5C3D-406A-9B7E-7D42DD381C89}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{658EC012-E050-42DC-B921-A2748A1BC13F}"/>
 </file>
</xml_diff>